<commit_message>
fix - stage bgm 변경
</commit_message>
<xml_diff>
--- a/Resource/DataTable/AllSoundList.xlsx
+++ b/Resource/DataTable/AllSoundList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2Q\2Q_AttackDefenceLog\Resource\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C0024F-2976-4FE9-8429-A5209EEA2D21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55837155-940E-4FF9-80EB-00E36837AD69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060" xr2:uid="{B78BD752-3219-4990-A2FB-AAA85CCD87BF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>SoundID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,86 +131,91 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>../../Resource/sounds/node/node_active_1.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../Resource/sounds/node/node_active_2.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../Resource/sounds/node/node_active_3.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../Resource/sounds/attack/attack_1.mp3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FMOD_DEFAULT | FMOD_LOOP_OFF</t>
   </si>
   <si>
-    <t>../../Resource/sounds/attack/attack_2.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/vigor/vigorbreak_1.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/defence/defence_1.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/defence/defence_2.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/button/button_click.wav</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/down/down.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/combo/combo_line.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/combo_end/combo_end.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/combo_charge/combo_charge.wav</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/parry/parry_1.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/parry/parry_2.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/parry/parry_3.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/hit/hit.wav</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/dodge/dodge_1.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/dodge/dodge_2.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/stage_1.mp3</t>
-  </si>
-  <si>
     <t>FMOD_CREATESTREAM | FMOD_LOOP_NORMAL</t>
   </si>
   <si>
-    <t>../../Resource/sounds/stage_2.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/stage_3_2.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/End_bgm.mp3</t>
-  </si>
-  <si>
-    <t>../../Resource/sounds/main_bgm.mp3</t>
+    <t>\..\Resource\sounds\attack\attack_1.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\attack\attack_2.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\vigor\vigorbreak_1.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\node\node_active_1.wav</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\node\node_active_2.wav</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\node\node_active_3.wav</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\defence\defence_1.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\defence\defence_2.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\button\button_click.wav</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\down\down.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\combo\combo_line.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\combo_end\combo_end.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\combo_charge\combo_charge.wav</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\parry\parry_1.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\parry\parry_2.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\parry\parry_3.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\hit\hit.wav</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\dodge\dodge_1.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\dodge\dodge_2.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\stage_1.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\stage_2.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\stage_3_2.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\End_bgm.mp3</t>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\main_bgm.mp3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\..\Resource\sounds\ui\Text_Stamp.mp3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Stamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -574,21 +579,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE1142E-9DB6-4837-BD85-9DB77A36AA9D}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
-    <col min="2" max="2" width="55.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" customWidth="1"/>
+    <col min="2" max="2" width="55.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,279 +604,290 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>52</v>
       </c>
-      <c r="C25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>53</v>
       </c>
-      <c r="C26" t="s">
-        <v>49</v>
+      <c r="C27" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>